<commit_message>
adding code for poster color dis and pdf for that
</commit_message>
<xml_diff>
--- a/analysis/time_avg_pilot.xlsx
+++ b/analysis/time_avg_pilot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiaskuehlwein/pm_color/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848A1C29-6292-F143-ADE9-BAF5926145C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09413E16-184E-DC40-8483-6FD6B218E6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="14800" xr2:uid="{F7A8C53D-62F3-474D-856C-CDF2FED7D69A}"/>
   </bookViews>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC215302-4163-914D-9A92-5509E7663915}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
         <v>9.3055555555555558E-2</v>
       </c>
       <c r="G2" s="3">
-        <v>134</v>
+        <v>40</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -523,7 +523,7 @@
         <v>2.7777777777777679E-2</v>
       </c>
       <c r="G3" s="3">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -544,7 +544,7 @@
         <v>3.5416666666666652E-2</v>
       </c>
       <c r="G4" s="3">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -565,7 +565,7 @@
         <v>4.0277777777777801E-2</v>
       </c>
       <c r="G5" s="3">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -586,7 +586,7 @@
         <v>2.3611111111111027E-2</v>
       </c>
       <c r="G6" s="3">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -607,7 +607,7 @@
         <v>3.9583333333333304E-2</v>
       </c>
       <c r="G7" s="3">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -628,7 +628,7 @@
         <v>4.9999999999999933E-2</v>
       </c>
       <c r="G8" s="3">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -649,7 +649,7 @@
         <v>3.2638888888888884E-2</v>
       </c>
       <c r="G9" s="3">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -670,7 +670,7 @@
         <v>3.9583333333333304E-2</v>
       </c>
       <c r="G10" s="3">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -691,7 +691,7 @@
         <v>2.9166666666666785E-2</v>
       </c>
       <c r="G11" s="3">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -712,7 +712,7 @@
         <v>3.7500000000000033E-2</v>
       </c>
       <c r="G12" s="3">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -733,7 +733,7 @@
         <v>2.777777777777779E-2</v>
       </c>
       <c r="G13" s="3">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -754,7 +754,7 @@
         <v>3.6805555555555536E-2</v>
       </c>
       <c r="G14" s="3">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -775,7 +775,7 @@
         <v>4.513888888888884E-2</v>
       </c>
       <c r="G15" s="3">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -795,11 +795,11 @@
         <f t="shared" si="0"/>
         <v>4.2361111111111072E-2</v>
       </c>
-      <c r="G16" s="3">
-        <v>61</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <f>STDEV(E2, E16)</f>
+        <v>3.5846385435151382E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>